<commit_message>
Pulled from master and added bus services info in html
</commit_message>
<xml_diff>
--- a/propertea/static/propertea.xlsx
+++ b/propertea/static/propertea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alice/PycharmProjects/propertea/propertea/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F42B594-9F68-3448-9F22-4E330AA3906F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B3DEDF-A558-9B43-B3C0-78E809217067}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16520" windowHeight="15120" xr2:uid="{A9FE1178-16BE-6F40-831E-B0E9FEA4E7EC}"/>
   </bookViews>
@@ -1002,7 +1002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89DCC537-74DB-C847-A2DD-CA8559776D68}">
   <dimension ref="A1:F86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="99" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
error notice for no search value and remove duplicate
</commit_message>
<xml_diff>
--- a/propertea/static/propertea.xlsx
+++ b/propertea/static/propertea.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alice/PycharmProjects/propertea/propertea/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B3DEDF-A558-9B43-B3C0-78E809217067}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EDF8F7-3798-474E-9A99-4A9C23FA4329}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16520" windowHeight="15120" xr2:uid="{A9FE1178-16BE-6F40-831E-B0E9FEA4E7EC}"/>
+    <workbookView xWindow="7660" yWindow="880" windowWidth="16520" windowHeight="15120" xr2:uid="{A9FE1178-16BE-6F40-831E-B0E9FEA4E7EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="188">
   <si>
     <t>DISTRICT</t>
   </si>
@@ -59,12 +62,6 @@
     <t xml:space="preserve">2 Marina Boulevard 018987 </t>
   </si>
   <si>
-    <t>Riviere</t>
-  </si>
-  <si>
-    <t>Jiak Kim Street 169000</t>
-  </si>
-  <si>
     <t>The Clift</t>
   </si>
   <si>
@@ -89,12 +86,6 @@
     <t>18 Spottiswoode Park Road 088642</t>
   </si>
   <si>
-    <t>Skysuites @ Anson</t>
-  </si>
-  <si>
-    <t>8 Enggor Street 079718</t>
-  </si>
-  <si>
     <t>Altez</t>
   </si>
   <si>
@@ -431,9 +422,6 @@
     <t>D07</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>99 Yishun Avenue 1 The Estuary Singapore 769139</t>
   </si>
   <si>
@@ -588,13 +576,37 @@
   </si>
   <si>
     <t>483 River Valley Road Valley Park Singapore 248368</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>D13</t>
+  </si>
+  <si>
+    <t>D15</t>
+  </si>
+  <si>
+    <t>D17</t>
+  </si>
+  <si>
+    <t>D18</t>
+  </si>
+  <si>
+    <t>D24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I need to add  this </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -652,6 +664,19 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFD5D5D5"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -674,7 +699,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -685,6 +710,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1000,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89DCC537-74DB-C847-A2DD-CA8559776D68}">
-  <dimension ref="A1:F86"/>
+  <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="99" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1012,6 +1039,7 @@
     <col min="2" max="2" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -1019,24 +1047,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -1056,7 +1084,7 @@
     </row>
     <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>6</v>
@@ -1074,9 +1102,9 @@
         <v>103.855507</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>5</v>
@@ -1087,24 +1115,36 @@
       <c r="D4" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E4" s="10">
+        <v>1.2793162059999901</v>
+      </c>
+      <c r="F4" s="10">
+        <v>103.850536099999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="E5" s="10">
+        <v>1.27940951</v>
+      </c>
+      <c r="F5" s="10">
+        <v>103.8473465</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -1115,12 +1155,18 @@
       <c r="D6" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="E6" s="10">
+        <v>1.277114649</v>
+      </c>
+      <c r="F6" s="10">
+        <v>103.84587449999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -1129,10 +1175,16 @@
       <c r="D7" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="E7" s="10">
+        <v>1.275163171</v>
+      </c>
+      <c r="F7" s="10">
+        <v>103.84448140000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>15</v>
@@ -1143,12 +1195,18 @@
       <c r="D8" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="E8" s="10">
+        <v>1.275567594</v>
+      </c>
+      <c r="F8" s="10">
+        <v>103.83759509999901</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -1157,38 +1215,56 @@
       <c r="D9" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="E9" s="10">
+        <v>1.274617941</v>
+      </c>
+      <c r="F9" s="10">
+        <v>103.84431960000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="E10" s="10">
+        <v>1.290736602</v>
+      </c>
+      <c r="F10" s="10">
+        <v>103.81806520000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="E11" s="10">
+        <v>1.2918914530000001</v>
+      </c>
+      <c r="F11" s="10">
+        <v>103.825380799999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>31</v>
@@ -1199,10 +1275,16 @@
       <c r="D12" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="E12" s="10">
+        <v>1.290385364</v>
+      </c>
+      <c r="F12" s="10">
+        <v>103.818982599999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>33</v>
@@ -1213,10 +1295,16 @@
       <c r="D13" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="E13" s="10">
+        <v>1.295566284</v>
+      </c>
+      <c r="F13" s="10">
+        <v>103.8062044</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>35</v>
@@ -1227,66 +1315,96 @@
       <c r="D14" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="E14" s="10">
+        <v>1.2928986520000001</v>
+      </c>
+      <c r="F14" s="10">
+        <v>103.8062224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="D15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="10">
+        <v>1.2439235959999999</v>
+      </c>
+      <c r="F15" s="10">
+        <v>103.8422557</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="B16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>38</v>
-      </c>
       <c r="D16" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="E16" s="10">
+        <v>1.2397701999999999</v>
+      </c>
+      <c r="F16" s="10">
+        <v>103.83409469999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B17" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="D17" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="E17" s="10">
+        <v>1.282649167</v>
+      </c>
+      <c r="F17" s="10">
+        <v>103.8031898</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="D18" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="10">
+        <v>1.245498258</v>
+      </c>
+      <c r="F18" s="10">
+        <v>103.8437327</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>47</v>
@@ -1297,38 +1415,56 @@
       <c r="D19" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="E19" s="10">
+        <v>1.266481065</v>
+      </c>
+      <c r="F19" s="10">
+        <v>103.8151282</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="D20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="10">
+        <v>1.295058713</v>
+      </c>
+      <c r="F20" s="10">
+        <v>103.7682344</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="B21" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="D21" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="E21" s="10">
+        <v>1.29727003</v>
+      </c>
+      <c r="F21" s="10">
+        <v>103.76517819999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>54</v>
@@ -1339,10 +1475,16 @@
       <c r="D22" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="E22" s="10">
+        <v>1.2937199150000001</v>
+      </c>
+      <c r="F22" s="10">
+        <v>103.76785049999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>56</v>
@@ -1353,10 +1495,16 @@
       <c r="D23" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="E23" s="10">
+        <v>1.3042854719999999</v>
+      </c>
+      <c r="F23" s="10">
+        <v>103.7837718</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>58</v>
@@ -1367,373 +1515,391 @@
       <c r="D24" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="7" t="s">
+      <c r="E24" s="10">
+        <v>1.3053716369999999</v>
+      </c>
+      <c r="F24" s="10">
+        <v>103.7882982</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="9">
+        <v>1.41104826332537</v>
+      </c>
+      <c r="F25" s="9">
+        <v>103.83251324502601</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>61</v>
+      <c r="B26" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" t="s">
+        <v>73</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>1</v>
+      </c>
+      <c r="E26" s="9">
+        <v>1.3961164823301899</v>
+      </c>
+      <c r="F26" s="9">
+        <v>103.874784556433</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E27" s="9">
-        <v>1.41104826332537</v>
+        <v>1.4272872745840099</v>
       </c>
       <c r="F27" s="9">
-        <v>103.83251324502601</v>
+        <v>103.786050332413</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
       <c r="C28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E28" s="9">
-        <v>1.3961164823301899</v>
+        <v>1.4381232559760899</v>
       </c>
       <c r="F28" s="9">
-        <v>103.874784556433</v>
+        <v>103.83122544979</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>134</v>
+        <v>76</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E29" s="9">
-        <v>1.4272872745840099</v>
+        <v>1.3937279859023799</v>
       </c>
       <c r="F29" s="9">
-        <v>103.786050332413</v>
+        <v>103.880812809353</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E30" s="9">
-        <v>1.4381232559760899</v>
+        <v>1.4321908361814699</v>
       </c>
       <c r="F30" s="9">
-        <v>103.83122544979</v>
+        <v>103.79745091654</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>80</v>
+        <v>132</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E31" s="9">
-        <v>1.3937279859023799</v>
+        <v>1.4436347320759899</v>
       </c>
       <c r="F31" s="9">
-        <v>103.880812809353</v>
+        <v>103.82525327968401</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E32" s="9">
-        <v>1.4321908361814699</v>
+        <v>1.39475153870194</v>
       </c>
       <c r="F32" s="9">
-        <v>103.79745091654</v>
+        <v>103.88175831363699</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>137</v>
+        <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E33" s="9">
-        <v>1.4436347320759899</v>
+        <v>1.4278629187293601</v>
       </c>
       <c r="F33" s="9">
-        <v>103.82525327968401</v>
+        <v>103.836107549028</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>138</v>
+        <v>81</v>
       </c>
       <c r="C34" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E34" s="9">
-        <v>1.39475153870194</v>
+        <v>1.44466302802823</v>
       </c>
       <c r="F34" s="9">
-        <v>103.88175831363699</v>
+        <v>103.824751090841</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>84</v>
+        <v>134</v>
       </c>
       <c r="C35" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E35" s="9">
-        <v>1.4278629187293601</v>
+        <v>1.44545498067156</v>
       </c>
       <c r="F35" s="9">
-        <v>103.836107549028</v>
+        <v>103.806251245325</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>85</v>
+        <v>135</v>
       </c>
       <c r="C36" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E36" s="9">
-        <v>1.44466302802823</v>
+        <v>1.3813560594127301</v>
       </c>
       <c r="F36" s="9">
-        <v>103.824751090841</v>
+        <v>103.827424659115</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C37" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E37" s="9">
-        <v>1.44545498067156</v>
+        <v>1.38224868339291</v>
       </c>
       <c r="F37" s="9">
-        <v>103.806251245325</v>
+        <v>103.836412663909</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>140</v>
+        <v>85</v>
       </c>
       <c r="C38" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E38" s="9">
-        <v>1.3813560594127301</v>
+        <v>1.4170896457081099</v>
       </c>
       <c r="F38" s="9">
-        <v>103.827424659115</v>
+        <v>103.848167820044</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C39" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E39" s="9">
-        <v>1.38224868339291</v>
+        <v>1.4132161422168401</v>
       </c>
       <c r="F39" s="9">
-        <v>103.836412663909</v>
+        <v>103.83484157476499</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>89</v>
+        <v>138</v>
       </c>
       <c r="C40" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E40" s="9">
-        <v>1.4170896457081099</v>
+        <v>1.3864321189461699</v>
       </c>
       <c r="F40" s="9">
-        <v>103.848167820044</v>
+        <v>103.84076155459201</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C41" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E41" s="9">
-        <v>1.4132161422168401</v>
+        <v>1.4183759609040301</v>
       </c>
       <c r="F41" s="9">
-        <v>103.83484157476499</v>
+        <v>103.84711068247699</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>143</v>
+        <v>89</v>
       </c>
       <c r="C42" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E42" s="9">
-        <v>1.3864321189461699</v>
+        <v>1.4351472525982001</v>
       </c>
       <c r="F42" s="9">
-        <v>103.84076155459201</v>
+        <v>103.844361011755</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C43" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E43" s="9">
-        <v>1.4183759609040301</v>
+        <v>1.4300288769068099</v>
       </c>
       <c r="F43" s="9">
-        <v>103.84711068247699</v>
+        <v>103.785578945342</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1741,219 +1907,219 @@
         <v>63</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>93</v>
+        <v>141</v>
       </c>
       <c r="C44" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E44" s="9">
-        <v>1.4351472525982001</v>
+        <v>1.3430039675551</v>
       </c>
       <c r="F44" s="9">
-        <v>103.844361011755</v>
+        <v>103.719009651994</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C45" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E45" s="9">
-        <v>1.4300288769068099</v>
+        <v>1.34280248734964</v>
       </c>
       <c r="F45" s="9">
-        <v>103.785578945342</v>
+        <v>103.718601989018</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C46" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E46" s="9">
-        <v>1.3430039675551</v>
+        <v>1.3456575114742699</v>
       </c>
       <c r="F46" s="9">
-        <v>103.719009651994</v>
+        <v>103.725314555002</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C47" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E47" s="9">
-        <v>1.34280248734964</v>
+        <v>1.3462606685352501</v>
       </c>
       <c r="F47" s="9">
-        <v>103.718601989018</v>
+        <v>103.722832489094</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C48" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E48" s="9">
-        <v>1.3456575114742699</v>
+        <v>1.34331070816855</v>
       </c>
       <c r="F48" s="9">
-        <v>103.725314555002</v>
+        <v>103.733218675595</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C49" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E49" s="9">
-        <v>1.3462606685352501</v>
+        <v>1.34005396911046</v>
       </c>
       <c r="F49" s="9">
-        <v>103.722832489094</v>
+        <v>103.705755724564</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C50" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E50" s="9">
-        <v>1.34331070816855</v>
+        <v>1.36546552129853</v>
       </c>
       <c r="F50" s="9">
-        <v>103.733218675595</v>
+        <v>103.771773342397</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C51" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E51" s="9">
-        <v>1.34005396911046</v>
+        <v>1.36908360324967</v>
       </c>
       <c r="F51" s="9">
-        <v>103.705755724564</v>
+        <v>103.777214643745</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C52" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E52" s="9">
-        <v>1.36546552129853</v>
+        <v>1.33297780085136</v>
       </c>
       <c r="F52" s="9">
-        <v>103.771773342397</v>
+        <v>103.787232054843</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C53" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E53" s="9">
-        <v>1.36908360324967</v>
+        <v>1.3362963694596499</v>
       </c>
       <c r="F53" s="9">
-        <v>103.777214643745</v>
+        <v>103.74173137219</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C54" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E54" s="9">
-        <v>1.33297780085136</v>
+        <v>1.3213814982746399</v>
       </c>
       <c r="F54" s="9">
-        <v>103.787232054843</v>
+        <v>103.86464484083901</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -1961,628 +2127,677 @@
         <v>67</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C55" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E55" s="9">
-        <v>1.3362963694596499</v>
+        <v>1.3518259898662699</v>
       </c>
       <c r="F55" s="9">
-        <v>103.74173137219</v>
+        <v>103.881368087162</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C56" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E56" s="9">
-        <v>1.3213814982746399</v>
+        <v>1.3519880092246199</v>
       </c>
       <c r="F56" s="9">
-        <v>103.86464484083901</v>
+        <v>103.852042784741</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C57" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E57" s="9">
-        <v>1.3518259898662699</v>
+        <v>1.30682843233651</v>
       </c>
       <c r="F57" s="9">
-        <v>103.881368087162</v>
+        <v>103.888972825423</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C58" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E58" s="9">
-        <v>1.3519880092246199</v>
+        <v>1.3126138404201599</v>
       </c>
       <c r="F58" s="9">
-        <v>103.852042784741</v>
+        <v>103.93933400726399</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C59" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E59" s="9">
-        <v>1.30682843233651</v>
+        <v>1.3920243070823799</v>
       </c>
       <c r="F59" s="9">
-        <v>103.888972825423</v>
+        <v>103.896214703952</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C60" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E60" s="9">
-        <v>1.3126138404201599</v>
+        <v>1.32767658775033</v>
       </c>
       <c r="F60" s="9">
-        <v>103.93933400726399</v>
+        <v>103.949805173068</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C61" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E61" s="9">
-        <v>1.3920243070823799</v>
+        <v>1.3784650059485299</v>
       </c>
       <c r="F61" s="9">
-        <v>103.896214703952</v>
+        <v>103.90252253712499</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C62" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E62" s="9">
-        <v>1.32767658775033</v>
+        <v>1.3755004316510899</v>
       </c>
       <c r="F62" s="9">
-        <v>103.949805173068</v>
+        <v>103.83442218814299</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C63" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E63" s="9">
-        <v>1.3784650059485299</v>
+        <v>1.36057979358354</v>
       </c>
       <c r="F63" s="9">
-        <v>103.90252253712499</v>
+        <v>103.88469543801</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C64" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E64" s="9">
-        <v>1.3755004316510899</v>
+        <v>1.31514292228326</v>
       </c>
       <c r="F64" s="9">
-        <v>103.83442218814299</v>
+        <v>103.80201123584</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>71</v>
+        <v>18</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C65" t="s">
-        <v>114</v>
+        <v>2</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E65" s="9">
-        <v>1.36057979358354</v>
+        <v>1.2807694347684899</v>
       </c>
       <c r="F65" s="9">
-        <v>103.88469543801</v>
+        <v>103.852658562152</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C66" t="s">
-        <v>115</v>
+        <v>42</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E66" s="9">
-        <v>1.31514292228326</v>
+        <v>1.28221769648724</v>
       </c>
       <c r="F66" s="9">
-        <v>103.80201123584</v>
+        <v>103.803662042285</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C67" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E67" s="9">
-        <v>1.2807694347684899</v>
+        <v>1.2672495484489199</v>
       </c>
       <c r="F67" s="9">
-        <v>103.852658562152</v>
+        <v>103.81099528789299</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C68" t="s">
-        <v>46</v>
+        <v>113</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E68" s="9">
-        <v>1.28221769648724</v>
+        <v>1.31846830438558</v>
       </c>
       <c r="F68" s="9">
-        <v>103.803662042285</v>
+        <v>103.761614078737</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C69" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E69" s="9">
-        <v>1.2672495484489199</v>
+        <v>1.26784881382911</v>
       </c>
       <c r="F69" s="9">
-        <v>103.81099528789299</v>
+        <v>103.814972113173</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>52</v>
+        <v>125</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C70" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E70" s="9">
-        <v>1.31846830438558</v>
+        <v>1.3106230842105799</v>
       </c>
       <c r="F70" s="9">
-        <v>103.761614078737</v>
+        <v>103.85708787979701</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C71" t="s">
-        <v>118</v>
+        <v>32</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E71" s="9">
-        <v>1.26784881382911</v>
+        <v>1.29546342917998</v>
       </c>
       <c r="F71" s="9">
-        <v>103.814972113173</v>
+        <v>103.806515780156</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>129</v>
+        <v>19</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C72" t="s">
-        <v>119</v>
+        <v>12</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E72" s="9">
-        <v>1.3106230842105799</v>
+        <v>1.2751700004148401</v>
       </c>
       <c r="F72" s="9">
-        <v>103.85708787979701</v>
+        <v>103.844496391516</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>29</v>
+        <v>126</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C73" t="s">
-        <v>36</v>
+        <v>116</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E73" s="9">
-        <v>1.29546342917998</v>
+        <v>1.29204842022799</v>
       </c>
       <c r="F73" s="9">
-        <v>103.806515780156</v>
+        <v>103.83639517422201</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C74" t="s">
-        <v>14</v>
+        <v>117</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E74" s="9">
-        <v>1.2751700004148401</v>
+        <v>1.29094473172583</v>
       </c>
       <c r="F74" s="9">
-        <v>103.844496391516</v>
+        <v>103.817000115258</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C75" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E75" s="9">
-        <v>1.29204842022799</v>
+        <v>1.29916295967818</v>
       </c>
       <c r="F75" s="9">
-        <v>103.83639517422201</v>
+        <v>103.857859536947</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>29</v>
+        <v>125</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C76" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E76" s="9">
-        <v>1.29094473172583</v>
+        <v>1.30899555275518</v>
       </c>
       <c r="F76" s="9">
-        <v>103.817000115258</v>
+        <v>103.862659611708</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>131</v>
+        <v>18</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C77" t="s">
-        <v>122</v>
+        <v>3</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E77" s="9">
-        <v>1.29916295967818</v>
+        <v>1.27722425616285</v>
       </c>
       <c r="F77" s="9">
-        <v>103.857859536947</v>
+        <v>103.853694940241</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>129</v>
+        <v>25</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C78" t="s">
-        <v>123</v>
+        <v>34</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E78" s="9">
-        <v>1.30899555275518</v>
+        <v>1.29267425406173</v>
       </c>
       <c r="F78" s="9">
-        <v>103.862659611708</v>
+        <v>103.806663243377</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>179</v>
+        <v>120</v>
       </c>
       <c r="C79" t="s">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E79" s="9">
-        <v>1.27722425616285</v>
+        <v>1.3134882244150901</v>
       </c>
       <c r="F79" s="9">
-        <v>103.853694940241</v>
+        <v>103.80169575460199</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>29</v>
+        <v>126</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C80" t="s">
-        <v>38</v>
+        <v>121</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E80" s="9">
-        <v>1.29267425406173</v>
+        <v>1.2947159593345099</v>
       </c>
       <c r="F80" s="9">
-        <v>103.806663243377</v>
+        <v>103.840051167364</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>124</v>
+        <v>177</v>
       </c>
       <c r="C81" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E81" s="9">
-        <v>1.3134882244150901</v>
+        <v>1.3149675067892199</v>
       </c>
       <c r="F81" s="9">
-        <v>103.80169575460199</v>
+        <v>103.75918294142799</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>130</v>
+        <v>18</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C82" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E82" s="9">
-        <v>1.2947159593345099</v>
+        <v>1.27962579891801</v>
       </c>
       <c r="F82" s="9">
-        <v>103.840051167364</v>
+        <v>103.854987203774</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C83" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E83" s="9">
-        <v>1.3149675067892199</v>
+        <v>1.29317347613803</v>
       </c>
       <c r="F83" s="9">
-        <v>103.75918294142799</v>
+        <v>103.828577644837</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>22</v>
+        <v>180</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C84" t="s">
-        <v>127</v>
+        <v>187</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>1</v>
-      </c>
-      <c r="E84" s="9">
-        <v>1.27962579891801</v>
-      </c>
-      <c r="F84" s="9">
-        <v>103.854987203774</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>75</v>
+        <v>182</v>
       </c>
       <c r="B85" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C85" t="s">
+        <v>187</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C86" t="s">
+        <v>187</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C87" t="s">
+        <v>187</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="C85" t="s">
-        <v>128</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E85" s="9">
-        <v>1.29317347613803</v>
-      </c>
-      <c r="F85" s="9">
-        <v>103.828577644837</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>132</v>
-      </c>
-      <c r="E86" t="str">
-        <f t="shared" ref="E86" si="0">PROPER(B86)</f>
-        <v/>
+      <c r="B88" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C88" t="s">
+        <v>187</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C89" t="s">
+        <v>187</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C90" t="s">
+        <v>187</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2590,5 +2805,6 @@
     <hyperlink ref="C2" r:id="rId1" display="https://www.edgeprop.sg/project/residential/the-sail-marina-bay-2199" xr:uid="{CED70BA7-8145-AA43-964F-FCFB53103424}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
some districts no property is it meant to be like that? (done)
</commit_message>
<xml_diff>
--- a/propertea/static/propertea.xlsx
+++ b/propertea/static/propertea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alice/PycharmProjects/propertea/propertea/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EDF8F7-3798-474E-9A99-4A9C23FA4329}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CBCA36-D712-8A4D-B083-A962534D6AD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7660" yWindow="880" windowWidth="16520" windowHeight="15120" xr2:uid="{A9FE1178-16BE-6F40-831E-B0E9FEA4E7EC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="238">
   <si>
     <t>DISTRICT</t>
   </si>
@@ -581,9 +581,6 @@
     <t>D11</t>
   </si>
   <si>
-    <t>Hello</t>
-  </si>
-  <si>
     <t>D13</t>
   </si>
   <si>
@@ -599,14 +596,167 @@
     <t>D24</t>
   </si>
   <si>
-    <t xml:space="preserve">I need to add  this </t>
+    <t>Lincoln Suites</t>
+  </si>
+  <si>
+    <t>3 Khiang Guan Avenue 308381</t>
+  </si>
+  <si>
+    <t>Neu At Novena</t>
+  </si>
+  <si>
+    <t>27 Moulmein Rise 308140</t>
+  </si>
+  <si>
+    <t>Daisy Petals</t>
+  </si>
+  <si>
+    <t>Barker Road</t>
+  </si>
+  <si>
+    <t>Mount Rosie Road</t>
+  </si>
+  <si>
+    <t>Daisy Avenue</t>
+  </si>
+  <si>
+    <t>Lynwood Grove</t>
+  </si>
+  <si>
+    <t>Sommerville Walk</t>
+  </si>
+  <si>
+    <t>Barker 9</t>
+  </si>
+  <si>
+    <t>Rosie View</t>
+  </si>
+  <si>
+    <t>Lynwood Eight</t>
+  </si>
+  <si>
+    <t>Fortune View</t>
+  </si>
+  <si>
+    <t>Sennett Residence</t>
+  </si>
+  <si>
+    <t>33 Pheng Geck Avenue 348228</t>
+  </si>
+  <si>
+    <t>Bartley Ridge</t>
+  </si>
+  <si>
+    <t>30 Mount Vernon Road 368055</t>
+  </si>
+  <si>
+    <t>Katong Regency</t>
+  </si>
+  <si>
+    <t>13 Tanjong Katong Road 437158</t>
+  </si>
+  <si>
+    <t>The Prominence</t>
+  </si>
+  <si>
+    <t>101 Haig Road 438749</t>
+  </si>
+  <si>
+    <t>Sunhaven</t>
+  </si>
+  <si>
+    <t>781 Upper Changi Road East 486069</t>
+  </si>
+  <si>
+    <t>Archipelago</t>
+  </si>
+  <si>
+    <t>Bedok Reservoir Road 470700</t>
+  </si>
+  <si>
+    <t>Azalea Park Condo</t>
+  </si>
+  <si>
+    <t>10 Flora Road 509729 Changi Airport </t>
+  </si>
+  <si>
+    <t>Parc Olympia</t>
+  </si>
+  <si>
+    <t>60 Flora Drive 506858</t>
+  </si>
+  <si>
+    <t>Coco Palms</t>
+  </si>
+  <si>
+    <t>Pasir Ris Grove 529999</t>
+  </si>
+  <si>
+    <t>My Manhattan</t>
+  </si>
+  <si>
+    <t>35 Simei Street 3 529904</t>
+  </si>
+  <si>
+    <t>Savannah Condopark</t>
+  </si>
+  <si>
+    <t>33 Simei Rise 528780</t>
+  </si>
+  <si>
+    <t>Mi Casa</t>
+  </si>
+  <si>
+    <t>321 321 Choa Chu Kang Avenue 3 689864</t>
+  </si>
+  <si>
+    <t>Casa Fidelio</t>
+  </si>
+  <si>
+    <t>Elite Court</t>
+  </si>
+  <si>
+    <t>East Tudor</t>
+  </si>
+  <si>
+    <t>Green Park</t>
+  </si>
+  <si>
+    <t>Loyang Court</t>
+  </si>
+  <si>
+    <t>Aston Residence</t>
+  </si>
+  <si>
+    <t>D'Elias</t>
+  </si>
+  <si>
+    <t>Fidelio Street</t>
+  </si>
+  <si>
+    <t>Elite Terrace (And 1 Others)</t>
+  </si>
+  <si>
+    <t>Upper Changi Road</t>
+  </si>
+  <si>
+    <t>Jalan Limau Kasturi</t>
+  </si>
+  <si>
+    <t>Jalan Loyang Besar 2</t>
+  </si>
+  <si>
+    <t>Jalan Loyang Besar</t>
+  </si>
+  <si>
+    <t>Elias Terrace</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -677,6 +827,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF2C2C2C"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -699,7 +861,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -712,6 +874,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1027,10 +1191,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89DCC537-74DB-C847-A2DD-CA8559776D68}">
-  <dimension ref="A1:F90"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="99" workbookViewId="0">
-      <selection activeCell="F86" sqref="F86"/>
+    <sheetView tabSelected="1" topLeftCell="D96" zoomScale="171" workbookViewId="0">
+      <selection activeCell="F109" sqref="F109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2642,7 +2806,7 @@
         <v>103.840051167364</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>48</v>
       </c>
@@ -2662,7 +2826,7 @@
         <v>103.75918294142799</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>18</v>
       </c>
@@ -2682,7 +2846,7 @@
         <v>103.854987203774</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>71</v>
       </c>
@@ -2702,105 +2866,640 @@
         <v>103.828577644837</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" ht="23" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>180</v>
       </c>
-      <c r="B84" s="9" t="s">
+      <c r="B84" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E84" s="9">
+        <v>1.317059531</v>
+      </c>
+      <c r="F84" s="10">
+        <v>103.8428088</v>
+      </c>
+      <c r="G84" t="str">
+        <f>_xlfn.CONCAT("'",C84,"',")</f>
+        <v>'Lincoln Suites',</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>180</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C85" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E85" s="9">
+        <v>1.3196337759999901</v>
+      </c>
+      <c r="F85" s="10">
+        <v>103.84598370000001</v>
+      </c>
+      <c r="G85" t="str">
+        <f t="shared" ref="G85:G109" si="0">_xlfn.CONCAT("'",C85,"',")</f>
+        <v>'Neu At Novena',</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>180</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C86" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E86" s="10">
+        <v>1.319949086</v>
+      </c>
+      <c r="F86" s="10">
+        <v>103.8338284</v>
+      </c>
+      <c r="G86" t="str">
+        <f t="shared" si="0"/>
+        <v>'Barker 9',</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>180</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C87" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E87" s="9">
+        <v>1.322525245</v>
+      </c>
+      <c r="F87" s="10">
+        <v>103.8357522</v>
+      </c>
+      <c r="G87" t="str">
+        <f t="shared" si="0"/>
+        <v>'Rosie View',</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>181</v>
       </c>
-      <c r="C84" t="s">
-        <v>187</v>
-      </c>
-      <c r="D84" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+      <c r="B88" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C88" t="s">
+        <v>190</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E88" s="10">
+        <v>1.3447967729999999</v>
+      </c>
+      <c r="F88" s="10">
+        <v>103.8675442</v>
+      </c>
+      <c r="G88" t="str">
+        <f t="shared" si="0"/>
+        <v>'Daisy Petals',</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>181</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C89" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E89" s="10">
+        <v>1.3450315450000001</v>
+      </c>
+      <c r="F89" s="10">
+        <v>103.863085599999</v>
+      </c>
+      <c r="G89" t="str">
+        <f t="shared" si="0"/>
+        <v>'Lynwood Eight',</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>181</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C90" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E90" s="10">
+        <v>1.346089885</v>
+      </c>
+      <c r="F90" s="10">
+        <v>103.8705355</v>
+      </c>
+      <c r="G90" t="str">
+        <f t="shared" si="0"/>
+        <v>'Fortune View',</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>181</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C91" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E91" s="10">
+        <v>1.3312352709999999</v>
+      </c>
+      <c r="F91" s="10">
+        <v>103.8695475</v>
+      </c>
+      <c r="G91" t="str">
+        <f t="shared" si="0"/>
+        <v>'Sennett Residence',</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>181</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="C92" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E92" s="10">
+        <v>1.340684309</v>
+      </c>
+      <c r="F92" s="10">
+        <v>103.8811104</v>
+      </c>
+      <c r="G92" t="str">
+        <f t="shared" si="0"/>
+        <v>'Bartley Ridge',</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A93" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="B85" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="C85" t="s">
-        <v>187</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="11" t="s">
+      <c r="B93" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C93" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E93" s="10">
+        <v>1.3199646199999999</v>
+      </c>
+      <c r="F93" s="10">
+        <v>103.9217518</v>
+      </c>
+      <c r="G93" t="str">
+        <f t="shared" si="0"/>
+        <v>'Casa Fidelio',</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A94" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C94" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E94" s="10">
+        <v>1.3166490259999999</v>
+      </c>
+      <c r="F94" s="10">
+        <v>103.9252382</v>
+      </c>
+      <c r="G94" t="str">
+        <f t="shared" si="0"/>
+        <v>'Elite Court',</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A95" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C95" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E95" s="10">
+        <v>1.3146281870000001</v>
+      </c>
+      <c r="F95" s="10">
+        <v>103.8947107</v>
+      </c>
+      <c r="G95" t="str">
+        <f t="shared" si="0"/>
+        <v>'Katong Regency',</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A96" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C96" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E96" s="10">
+        <v>1.3106093679999999</v>
+      </c>
+      <c r="F96" s="10">
+        <v>103.89761439999999</v>
+      </c>
+      <c r="G96" t="str">
+        <f t="shared" si="0"/>
+        <v>'The Prominence',</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A97" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C97" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E97" s="10">
+        <v>1.3306085540000001</v>
+      </c>
+      <c r="F97" s="10">
+        <v>103.9446392</v>
+      </c>
+      <c r="G97" t="str">
+        <f t="shared" si="0"/>
+        <v>'East Tudor',</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A98" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C98" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E98" s="10">
+        <v>1.34758949199999</v>
+      </c>
+      <c r="F98" s="10">
+        <v>103.7881737</v>
+      </c>
+      <c r="G98" t="str">
+        <f t="shared" si="0"/>
+        <v>'Green Park',</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A99" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C99" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E99" s="10">
+        <v>1.34804103199999</v>
+      </c>
+      <c r="F99" s="10">
+        <v>103.9618747</v>
+      </c>
+      <c r="G99" t="str">
+        <f t="shared" si="0"/>
+        <v>'Sunhaven',</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A100" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C100" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E100" s="10">
+        <v>1.3384713100000001</v>
+      </c>
+      <c r="F100" s="10">
+        <v>103.9198304</v>
+      </c>
+      <c r="G100" t="str">
+        <f t="shared" si="0"/>
+        <v>'Archipelago',</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A101" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="B86" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="C86" t="s">
-        <v>187</v>
-      </c>
-      <c r="D86" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B87" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="C87" t="s">
-        <v>187</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="11" t="s">
+      <c r="B101" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C101" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E101" s="10">
+        <v>1.3785630200000001</v>
+      </c>
+      <c r="F101" s="10">
+        <v>103.95951289999999</v>
+      </c>
+      <c r="G101" t="str">
+        <f t="shared" si="0"/>
+        <v>'Loyang Court',</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A102" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C102" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E102" s="10">
+        <v>1.3801562249999999</v>
+      </c>
+      <c r="F102" s="10">
+        <v>103.96445370000001</v>
+      </c>
+      <c r="G102" t="str">
+        <f t="shared" si="0"/>
+        <v>'Aston Residence',</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A103" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="B103" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C103" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E103" s="10">
+        <v>1.3604258890000001</v>
+      </c>
+      <c r="F103" s="10">
+        <v>103.9627309</v>
+      </c>
+      <c r="G103" t="str">
+        <f t="shared" si="0"/>
+        <v>'Azalea Park Condo',</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A104" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="B104" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="C104" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E104" s="10">
+        <v>1.3553987329999999</v>
+      </c>
+      <c r="F104" s="10">
+        <v>103.964723599999</v>
+      </c>
+      <c r="G104" t="str">
+        <f t="shared" si="0"/>
+        <v>'Parc Olympia',</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A105" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="B88" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="C88" t="s">
-        <v>187</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="11" t="s">
+      <c r="B105" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C105" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E105" s="10">
+        <v>1.3728458559999901</v>
+      </c>
+      <c r="F105" s="10">
+        <v>103.9413845</v>
+      </c>
+      <c r="G105" t="str">
+        <f t="shared" si="0"/>
+        <v>'D'Elias',</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A106" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="B106" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="C106" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E106" s="10">
+        <v>1.3717436240000001</v>
+      </c>
+      <c r="F106" s="10">
+        <v>103.9459262</v>
+      </c>
+      <c r="G106" t="str">
+        <f t="shared" si="0"/>
+        <v>'Coco Palms',</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A107" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="C107" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E107" s="10">
+        <v>1.3416932420000001</v>
+      </c>
+      <c r="F107" s="10">
+        <v>103.95370759999901</v>
+      </c>
+      <c r="G107" t="str">
+        <f t="shared" si="0"/>
+        <v>'My Manhattan',</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A108" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="B108" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="C108" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E108" s="10">
+        <v>1.3492793890000001</v>
+      </c>
+      <c r="F108" s="10">
+        <v>103.96161770000001</v>
+      </c>
+      <c r="G108" t="str">
+        <f t="shared" si="0"/>
+        <v>'Savannah Condopark',</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A109" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="B89" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="C89" t="s">
-        <v>187</v>
-      </c>
-      <c r="D89" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="B90" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="C90" t="s">
-        <v>187</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="B109" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="C109" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E109" s="10">
+        <v>1.3841914639999999</v>
+      </c>
+      <c r="F109" s="10">
+        <v>103.7480539</v>
+      </c>
+      <c r="G109" t="str">
+        <f t="shared" si="0"/>
+        <v>'Mi Casa',</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A110" s="11"/>
+      <c r="D110" s="5"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A111" s="11"/>
+      <c r="D111" s="5"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="https://www.edgeprop.sg/project/residential/the-sail-marina-bay-2199" xr:uid="{CED70BA7-8145-AA43-964F-FCFB53103424}"/>
   </hyperlinks>

</xml_diff>